<commit_message>
Incorporate all modules into main directory, update Final-Project-Plan and Final-Project_Test_Cases
</commit_message>
<xml_diff>
--- a/V3/Final-Project-Plan.xlsx
+++ b/V3/Final-Project-Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/adsmith6_myseneca_ca/Documents/CPR101/finalProject/project/git/CPR101group3/V2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/adsmith6_myseneca_ca/Documents/CPR101/finalProject/project/V3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{40108199-1571-4FD1-AE3A-D7CA79A9ACE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8A311EC-A2FB-4286-8E3C-D9AE24553BF7}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{40108199-1571-4FD1-AE3A-D7CA79A9ACE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27A60A44-5461-4AB6-B6A8-05374A234B1F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D8E31B3C-F149-45D6-99B7-2CDC65D256FF}"/>
   </bookViews>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>Blackboard Group No
 3 Class NAA</t>
@@ -1219,6 +1219,18 @@
   </si>
   <si>
     <t>Add converting to doubles module and push to github, add all other modules to main and push to github.</t>
+  </si>
+  <si>
+    <t>Add converting to long module, push to github, add zip file to teams, compile all to final version for github, teams and blackboard</t>
+  </si>
+  <si>
+    <t>final tests all pass</t>
+  </si>
+  <si>
+    <t>Add searching strings demo and push to github, send to teams</t>
+  </si>
+  <si>
+    <t>manipulations tests pass</t>
   </si>
 </sst>
 </file>
@@ -2356,10 +2368,10 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="N8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P11" sqref="P11"/>
+      <selection pane="bottomRight" activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,11 +2394,11 @@
     <col min="16" max="16" width="12.140625" style="19" customWidth="1"/>
     <col min="17" max="17" width="25.7109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="28.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.7109375" style="19" customWidth="1"/>
     <col min="21" max="21" width="12.140625" style="19" customWidth="1"/>
     <col min="22" max="23" width="25.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.7109375" style="19" customWidth="1"/>
     <col min="26" max="26" width="12.140625" style="19" customWidth="1"/>
     <col min="27" max="16384" width="9.140625" style="1"/>
@@ -2748,7 +2760,7 @@
 Dec.12</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>35</v>
@@ -2756,7 +2768,9 @@
       <c r="W5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="X5" s="12"/>
+      <c r="X5" s="12">
+        <v>42</v>
+      </c>
       <c r="Y5" s="23" t="str">
         <f>IF(($W$3+Y$3-2)&lt;$W$3,(TEXT(($W$3+Y$3-2),"dddd
 ") &amp; TEXT(($W$3+Y$3-2),"mmm.d")),(TEXT($W$3,"dddd
@@ -2765,7 +2779,7 @@
 Dec.12</v>
       </c>
       <c r="Z5" s="9" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2976,18 +2990,24 @@
       <c r="P8" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
+      <c r="Q8" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="S8" s="17">
+        <v>1</v>
+      </c>
       <c r="T8" s="23" t="str">
         <f>TEXT(($E$3+T$3-1),"dddd
 ") &amp; TEXT(($E$3+T$3-1),"mmm.d")</f>
         <v>Tuesday
 Dec.13</v>
       </c>
-      <c r="U8" s="17"/>
+      <c r="U8" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="V8" s="17"/>
       <c r="W8" s="17"/>
       <c r="X8" s="17"/>
@@ -3134,21 +3154,29 @@
       <c r="P10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
+      <c r="Q10" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="S10" s="11">
+        <v>2</v>
+      </c>
       <c r="T10" s="24" t="str">
         <f>TEXT(($E$3+T$3),"dddd
 ") &amp; TEXT(($E$3+T$3),"mmm.d")</f>
         <v>Wednesday
 Dec.14</v>
       </c>
-      <c r="U10" s="17"/>
+      <c r="U10" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="V10" s="17"/>
       <c r="W10" s="17"/>
-      <c r="X10" s="17"/>
+      <c r="X10" s="17">
+        <v>11</v>
+      </c>
       <c r="Y10" s="26" t="str">
         <f>IF(WORKDAY($W$3,Y$3)&lt;$W$3,(TEXT(WORKDAY($W$3,Y$3),"dddd
 ") &amp; TEXT(WORKDAY($W$3,Y$3),"mmm.d")),(TEXT($W$3,"dddd
@@ -3156,7 +3184,9 @@
         <v>Wednesday
 Dec.14</v>
       </c>
-      <c r="Z10" s="11"/>
+      <c r="Z10" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:26" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" s="22" t="s">
@@ -3364,6 +3394,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B0151594D7FCB5488E5A9E489924D9EC" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="782c9240cb3ad67681d064f8c60b5904">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="704fc4e2-c222-4319-b029-9522ae630171" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb47d0c3166dea3cfdc3792473b57f5a" ns2:_="">
     <xsd:import namespace="704fc4e2-c222-4319-b029-9522ae630171"/>
@@ -3501,22 +3546,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76FEA26C-2233-4295-8BE1-B265CEAD26C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A37522F-39F4-4439-AEEC-7D6E0C35C759}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{877BC3CA-6C3C-4A4E-AA42-8A543635C4C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3532,21 +3579,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A37522F-39F4-4439-AEEC-7D6E0C35C759}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76FEA26C-2233-4295-8BE1-B265CEAD26C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>